<commit_message>
2025.6.25 ItTeacher end over
</commit_message>
<xml_diff>
--- a/批量导入模板/基础设置模板/考核部门模板.xlsx
+++ b/批量导入模板/基础设置模板/考核部门模板.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\05 教学教研\2025学校网站开发\批量导入模板\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myGithub\ynyzjs\teacher_system\批量导入模板\基础设置模板\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BEEC10-993F-433E-876B-0A2DEE668821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978D18DC-847E-4858-8C40-97D8EEA25B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12000" yWindow="390" windowWidth="14670" windowHeight="15090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="1110" windowWidth="28260" windowHeight="15090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,10 +83,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>美术（书法）教师</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>体育教师</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -100,6 +96,10 @@
   </si>
   <si>
     <t>行政后勤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>美术教师</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -428,7 +428,7 @@
   <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -508,27 +508,27 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>